<commit_message>
suggested speed and block length
</commit_message>
<xml_diff>
--- a/CTC/Schedule_v2.xlsx
+++ b/CTC/Schedule_v2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\Documents\Pitt\2017 Fall Term\Lectures\Lecture 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{54806B6C-8A74-4C52-8AF2-CDA9DCC1B936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E868215-42D8-43DE-8671-7112FF61C9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="140" windowWidth="13380" windowHeight="6330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,70 +50,70 @@
     <t>Red</t>
   </si>
   <si>
-    <t>STATION; SHADYSIDE</t>
-  </si>
-  <si>
-    <t>STATION; HERRON AVE</t>
-  </si>
-  <si>
-    <t>STATION; SWISSVILLE</t>
-  </si>
-  <si>
-    <t>STATION; PENN STATION; UNDERGROUND</t>
-  </si>
-  <si>
-    <t>STATION; STEEL PLAZA; UNDERGROUND</t>
-  </si>
-  <si>
-    <t>STATION; FIRST; AVE; UNDERGROUND</t>
-  </si>
-  <si>
-    <t>STATION; STATION SQUARE</t>
-  </si>
-  <si>
-    <t>STATION; SOUTH HILLS JUNCTION</t>
+    <t>STATION; Shadyside</t>
+  </si>
+  <si>
+    <t>STATION; Herron_Ave</t>
+  </si>
+  <si>
+    <t>STATION; Swissville</t>
+  </si>
+  <si>
+    <t>STATION; Penn_Station UNDERGROUND</t>
+  </si>
+  <si>
+    <t>STATION; Steel_Plaza UNDERGROUND</t>
+  </si>
+  <si>
+    <t>STATION; First_Ave; UNDERGROUND</t>
+  </si>
+  <si>
+    <t>STATION; Station_Square</t>
+  </si>
+  <si>
+    <t>STATION; South_Hills_Junction</t>
   </si>
   <si>
     <t>Green</t>
   </si>
   <si>
-    <t>STATION; PIONEER</t>
-  </si>
-  <si>
-    <t>STATION; EDGEBROOK</t>
-  </si>
-  <si>
-    <t>STATION</t>
-  </si>
-  <si>
-    <t>STATION; WHITED</t>
-  </si>
-  <si>
-    <t>STATION; SOUTH BANK</t>
-  </si>
-  <si>
-    <t>STATION; CENTRAL; UNDERGROUND</t>
-  </si>
-  <si>
-    <t>STATION; INGLEWOOD; UNDERGROUND</t>
-  </si>
-  <si>
-    <t>STATION; GLENBURY</t>
-  </si>
-  <si>
-    <t>STATION; DORMONT</t>
-  </si>
-  <si>
-    <t>STATION; MT LEBANON</t>
-  </si>
-  <si>
-    <t>STATION; POPLAR</t>
-  </si>
-  <si>
-    <t>STATION; CASTLE SHANNON</t>
-  </si>
-  <si>
-    <t>STATION; OVERBROOK; UNDERGROUND</t>
+    <t>STATION; Pioneer</t>
+  </si>
+  <si>
+    <t>STATION; Edgebrook</t>
+  </si>
+  <si>
+    <t>STATION; Station</t>
+  </si>
+  <si>
+    <t>STATION; Whited</t>
+  </si>
+  <si>
+    <t>STATION; South_Bank</t>
+  </si>
+  <si>
+    <t>STATION; Central; UNDERGROUND</t>
+  </si>
+  <si>
+    <t>STATION; Inglewood; UNDERGROUND</t>
+  </si>
+  <si>
+    <t>STATION; Glenbury</t>
+  </si>
+  <si>
+    <t>STATION; Dormont</t>
+  </si>
+  <si>
+    <t>STATION; Mt_Lebanon</t>
+  </si>
+  <si>
+    <t>STATION; Poplar</t>
+  </si>
+  <si>
+    <t>STATION; Castle_Shannon</t>
+  </si>
+  <si>
+    <t>STATION; Overbrook; UNDERGROUND</t>
   </si>
 </sst>
 </file>
@@ -170,7 +170,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -492,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>

</xml_diff>